<commit_message>
Adding configs 4 me + update utils,Readme for config part + test write
</commit_message>
<xml_diff>
--- a/sample/saveconfig.xlsx
+++ b/sample/saveconfig.xlsx
@@ -130,7 +130,7 @@
     <t xml:space="preserve">audio_base_cluster</t>
   </si>
   <si>
-    <t xml:space="preserve">/NOT-REALLY</t>
+    <t xml:space="preserve">/NOT-IMPLEMENT-YET</t>
   </si>
   <si>
     <t xml:space="preserve">band1</t>
@@ -636,11 +636,11 @@
   </sheetPr>
   <dimension ref="A1:Y530"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U5" activeCellId="0" sqref="U5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.14"/>
@@ -3218,8 +3218,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>